<commit_message>
Correction to transportation files for shipping (removing bunkers)
</commit_message>
<xml_diff>
--- a/InputData/trans/BAADTbVT/BAU AvgAnnual Dist Traveled by Veh Type.xlsx
+++ b/InputData/trans/BAADTbVT/BAU AvgAnnual Dist Traveled by Veh Type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_Artelys/trans/BAADTbVT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\trans\BAADTbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{79C8DA45-06D6-4DCA-B929-0C94ED24A24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF355B04-CF39-4D07-9563-C46C0550E3F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ECC07D-89A6-4DF8-B7CE-24FBAFD7FA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="10" xr2:uid="{BB1BC0E8-D7BE-4817-AFF2-63D73B602A09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{BB1BC0E8-D7BE-4817-AFF2-63D73B602A09}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1145,9 +1145,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1185,7 +1185,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1291,7 +1291,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1433,7 +1433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1443,7 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964DB6D4-E3BC-4210-972A-F4C8906F80D5}">
   <dimension ref="B11:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2452,8 +2452,8 @@
   </sheetPr>
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3081,127 +3081,127 @@
       </c>
       <c r="B6" s="69">
         <f>Freight_km!B6*About!$C$21</f>
-        <v>98828.972390853916</v>
+        <v>94467.07984962406</v>
       </c>
       <c r="C6" s="69">
         <f>Freight_km!C6*About!$C$21</f>
-        <v>98772.228999615982</v>
+        <v>94465.627990225519</v>
       </c>
       <c r="D6" s="69">
         <f>Freight_km!D6*About!$C$21</f>
-        <v>98712.51782304942</v>
+        <v>94419.265234374994</v>
       </c>
       <c r="E6" s="69">
         <f>Freight_km!E6*About!$C$21</f>
-        <v>98700.839443435645</v>
+        <v>94478.337590361465</v>
       </c>
       <c r="F6" s="69">
         <f>Freight_km!F6*About!$C$21</f>
-        <v>98676.915097585254</v>
+        <v>94521.763960545781</v>
       </c>
       <c r="G6" s="69">
         <f>Freight_km!G6*About!$C$21</f>
-        <v>98714.6801905764</v>
+        <v>94608.557243650052</v>
       </c>
       <c r="H6" s="69">
         <f>Freight_km!H6*About!$C$21</f>
-        <v>98779.744517672603</v>
+        <v>94737.401767441857</v>
       </c>
       <c r="I6" s="69">
         <f>Freight_km!I6*About!$C$21</f>
-        <v>98895.560608846747</v>
+        <v>94935.626953600338</v>
       </c>
       <c r="J6" s="69">
         <f>Freight_km!J6*About!$C$21</f>
-        <v>98993.704507445</v>
+        <v>95129.749635701271</v>
       </c>
       <c r="K6" s="69">
         <f>Freight_km!K6*About!$C$21</f>
-        <v>99061.184850853882</v>
+        <v>95276.886666666673</v>
       </c>
       <c r="L6" s="69">
         <f>Freight_km!L6*About!$C$21</f>
-        <v>99210.868186779218</v>
+        <v>95533.688184746177</v>
       </c>
       <c r="M6" s="69">
         <f>Freight_km!M6*About!$C$21</f>
-        <v>99372.467967495089</v>
+        <v>95758.125762707481</v>
       </c>
       <c r="N6" s="69">
         <f>Freight_km!N6*About!$C$21</f>
-        <v>99486.483055019155</v>
+        <v>95963.374376912994</v>
       </c>
       <c r="O6" s="69">
         <f>Freight_km!O6*About!$C$21</f>
-        <v>99573.020259255602</v>
+        <v>96101.071868227111</v>
       </c>
       <c r="P6" s="69">
         <f>Freight_km!P6*About!$C$21</f>
-        <v>99678.897930094827</v>
+        <v>96195.06374570448</v>
       </c>
       <c r="Q6" s="69">
         <f>Freight_km!Q6*About!$C$21</f>
-        <v>99745.209353318322</v>
+        <v>96313.827628778192</v>
       </c>
       <c r="R6" s="69">
         <f>Freight_km!R6*About!$C$21</f>
-        <v>99814.703397343954</v>
+        <v>96416.000106755615</v>
       </c>
       <c r="S6" s="69">
         <f>Freight_km!S6*About!$C$21</f>
-        <v>99843.70722655172</v>
+        <v>96490.373422482255</v>
       </c>
       <c r="T6" s="69">
         <f>Freight_km!T6*About!$C$21</f>
-        <v>99949.416647532111</v>
+        <v>96692.017308488605</v>
       </c>
       <c r="U6" s="69">
         <f>Freight_km!U6*About!$C$21</f>
-        <v>99980.037370316364</v>
+        <v>96788.031021748058</v>
       </c>
       <c r="V6" s="69">
         <f>Freight_km!V6*About!$C$21</f>
-        <v>100040.39787256003</v>
+        <v>96904.587484762291</v>
       </c>
       <c r="W6" s="69">
         <f>Freight_km!W6*About!$C$21</f>
-        <v>100118.18943576055</v>
+        <v>97043.897424547278</v>
       </c>
       <c r="X6" s="69">
         <f>Freight_km!X6*About!$C$21</f>
-        <v>100179.85950714006</v>
+        <v>97166.58067729084</v>
       </c>
       <c r="Y6" s="69">
         <f>Freight_km!Y6*About!$C$21</f>
-        <v>100246.3695970374</v>
+        <v>97286.844142011832</v>
       </c>
       <c r="Z6" s="69">
         <f>Freight_km!Z6*About!$C$21</f>
-        <v>100339.67848222077</v>
+        <v>97377.227361436395</v>
       </c>
       <c r="AA6" s="69">
         <f>Freight_km!AA6*About!$C$21</f>
-        <v>100402.94021614488</v>
+        <v>97489.725840092709</v>
       </c>
       <c r="AB6" s="69">
         <f>Freight_km!AB6*About!$C$21</f>
-        <v>100437.02446622032</v>
+        <v>97535.554830087844</v>
       </c>
       <c r="AC6" s="69">
         <f>Freight_km!AC6*About!$C$21</f>
-        <v>100504.82942890898</v>
+        <v>97640.662046827812</v>
       </c>
       <c r="AD6" s="69">
         <f>Freight_km!AD6*About!$C$21</f>
-        <v>100558.39384351562</v>
+        <v>97697.049078929485</v>
       </c>
       <c r="AE6" s="69">
         <f>Freight_km!AE6*About!$C$21</f>
-        <v>100609.70133253871</v>
+        <v>97762.064610269677</v>
       </c>
       <c r="AF6" s="69">
         <f>Freight_km!AF6*About!$C$21</f>
-        <v>100635.44386879263</v>
+        <v>97802.93270003653</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -55544,7 +55544,7 @@
   <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56172,128 +56172,128 @@
         <v>114</v>
       </c>
       <c r="B6" s="82">
-        <f>B35</f>
-        <v>159049.86294959681</v>
+        <f>B33</f>
+        <v>152030.07518796992</v>
       </c>
       <c r="C6" s="82">
-        <f t="shared" ref="C6:AF6" si="1">C35</f>
-        <v>158958.54328511626</v>
+        <f t="shared" ref="C6:AF6" si="1">C33</f>
+        <v>152027.73864603517</v>
       </c>
       <c r="D6" s="82">
         <f t="shared" si="1"/>
-        <v>158862.44743164617</v>
+        <v>151953.125</v>
       </c>
       <c r="E6" s="82">
         <f t="shared" si="1"/>
-        <v>158843.65289567044</v>
+        <v>152048.19277108437</v>
       </c>
       <c r="F6" s="82">
         <f t="shared" si="1"/>
-        <v>158805.15038131044</v>
+        <v>152118.08076100395</v>
       </c>
       <c r="G6" s="82">
         <f t="shared" si="1"/>
-        <v>158865.92742592815</v>
+        <v>152257.76105362183</v>
       </c>
       <c r="H6" s="82">
         <f t="shared" si="1"/>
-        <v>158970.6383427495</v>
+        <v>152465.11627906977</v>
       </c>
       <c r="I6" s="82">
         <f t="shared" si="1"/>
-        <v>159157.02633184803</v>
+        <v>152784.12889175763</v>
       </c>
       <c r="J6" s="82">
         <f t="shared" si="1"/>
-        <v>159314.97367505886</v>
+        <v>153096.53916211292</v>
       </c>
       <c r="K6" s="82">
         <f t="shared" si="1"/>
-        <v>159423.57279443985</v>
+        <v>153333.33333333334</v>
       </c>
       <c r="L6" s="82">
         <f t="shared" si="1"/>
-        <v>159664.46484753749</v>
+        <v>153746.61544350506</v>
       </c>
       <c r="M6" s="82">
         <f t="shared" si="1"/>
-        <v>159924.53456549323</v>
+        <v>154107.8128247174</v>
       </c>
       <c r="N6" s="82">
         <f t="shared" si="1"/>
-        <v>160108.02411927682</v>
+        <v>154438.12855268913</v>
       </c>
       <c r="O6" s="82">
         <f t="shared" si="1"/>
-        <v>160247.29229277774</v>
+        <v>154659.73125270911</v>
       </c>
       <c r="P6" s="82">
         <f t="shared" si="1"/>
-        <v>160417.68593979254</v>
+        <v>154810.99656357389</v>
       </c>
       <c r="Q6" s="82">
         <f t="shared" si="1"/>
-        <v>160524.40386390468</v>
+        <v>155002.12856534694</v>
       </c>
       <c r="R6" s="82">
         <f t="shared" si="1"/>
-        <v>160636.24372129363</v>
+        <v>155166.55928061594</v>
       </c>
       <c r="S6" s="82">
         <f t="shared" si="1"/>
-        <v>160682.92087424698</v>
+        <v>155286.25156707063</v>
       </c>
       <c r="T6" s="82">
         <f t="shared" si="1"/>
-        <v>160853.04374927719</v>
+        <v>155610.76604554863</v>
       </c>
       <c r="U6" s="82">
         <f t="shared" si="1"/>
-        <v>160902.32304101152</v>
+        <v>155765.28518670498</v>
       </c>
       <c r="V6" s="82">
         <f t="shared" si="1"/>
-        <v>160999.46388318739</v>
+        <v>155952.86468915074</v>
       </c>
       <c r="W6" s="82">
         <f t="shared" si="1"/>
-        <v>161124.6573074066</v>
+        <v>156177.06237424546</v>
       </c>
       <c r="X6" s="82">
         <f t="shared" si="1"/>
-        <v>161223.90569746587</v>
+        <v>156374.50199203187</v>
       </c>
       <c r="Y6" s="82">
         <f t="shared" si="1"/>
-        <v>161330.94334469648</v>
+        <v>156568.04733727811</v>
       </c>
       <c r="Z6" s="82">
         <f t="shared" si="1"/>
-        <v>161481.10948567084</v>
+        <v>156713.50507416084</v>
       </c>
       <c r="AA6" s="82">
         <f t="shared" si="1"/>
-        <v>161582.91940908873</v>
+        <v>156894.55388180766</v>
       </c>
       <c r="AB6" s="82">
         <f t="shared" si="1"/>
-        <v>161637.77270941244</v>
+        <v>156968.3085147003</v>
       </c>
       <c r="AC6" s="82">
         <f t="shared" si="1"/>
-        <v>161746.89425304526</v>
+        <v>157137.46223564958</v>
       </c>
       <c r="AD6" s="82">
         <f t="shared" si="1"/>
-        <v>161833.09784897527</v>
+        <v>157228.2083955149</v>
       </c>
       <c r="AE6" s="82">
         <f t="shared" si="1"/>
-        <v>161915.66927413526</v>
+        <v>157332.8407831548</v>
       </c>
       <c r="AF6" s="82">
         <f t="shared" si="1"/>
-        <v>161957.09788321733</v>
+        <v>157398.61161856045</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -58615,8 +58615,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58671,7 +58671,7 @@
       </c>
       <c r="B6" s="69">
         <f>'BAADTbVT-freight'!C6</f>
-        <v>98772.228999615982</v>
+        <v>94465.627990225519</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -58700,6 +58700,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aabc5cd2cd094c10559845ba515387e4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="797afa85599b0f8981d985a9380993ae" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -58928,15 +58937,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E81C7721-51FE-4B65-A133-A786E226EB0D}">
   <ds:schemaRefs>
@@ -58949,6 +58949,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43343079-DE8F-4311-9B51-F202091843AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{657F731C-A1B4-47FF-936A-4B6BCF428667}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58965,12 +58973,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43343079-DE8F-4311-9B51-F202091843AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>